<commit_message>
123 - Rework new project page/comtroller ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=123 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/Requirements and FIT criteria.xlsx
+++ b/italent/documents/analyse/Requirements and FIT criteria.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t>Projectenlijst sorteren</t>
   </si>
@@ -123,24 +123,9 @@
     <t>De ingelogde gebruiker zal bestaan binnen het systeem</t>
   </si>
   <si>
-    <t>Het inloggen en de applicatie opstarten samen mag maximaal 2 seconden duren op eender welk device</t>
-  </si>
-  <si>
     <t>Indien er foute gegevens werden ingevoerd moet een duidelijke boodschap dit overbrengen</t>
   </si>
   <si>
-    <t>Het ophalen van de projectenlijst mag maximaal 2 seconden duren</t>
-  </si>
-  <si>
-    <t>Een gast kan tot 50 publieke projecten bekijken per pagina</t>
-  </si>
-  <si>
-    <t>Een student kan tot 50 gebackte projecten bekijken per pagina</t>
-  </si>
-  <si>
-    <t>Een docent kan tot 50 projecten bekijken per pagina</t>
-  </si>
-  <si>
     <t>Sorteren kan op basis van aantal likes: oplopend eerst</t>
   </si>
   <si>
@@ -171,21 +156,12 @@
     <t>Een gebruiker kan een project slechts 1 keer liken</t>
   </si>
   <si>
-    <t>Gebruikers moeten visueel makkelijk kunnen zien dat ze een project hebben geliked</t>
-  </si>
-  <si>
     <t>Enkel ingelogde gebruikers kunnen projectdetails opvragen</t>
   </si>
   <si>
     <t>Het opvragen van de details mag maximaal 2 seconden duren</t>
   </si>
   <si>
-    <t>Via de detailpagina moeten gebruikers binnen 10 seconden een korte beschrijving kunnen geven over de inhoud</t>
-  </si>
-  <si>
-    <t>De detailpagina moet duidelijk weergeven om welk domein het project betrekking heeft</t>
-  </si>
-  <si>
     <t>Fotos, videos en andere media dienen nooit meer dan 50 pct van de gehele schermruimte in beslag te nemen</t>
   </si>
   <si>
@@ -346,6 +322,27 @@
   </si>
   <si>
     <t>Het wissel van een pagina door gebruik te maken van het menu mag maximaal 2 seconden duren</t>
+  </si>
+  <si>
+    <t>Het inloggen en de applicatie opstarten samen mag maximaal 30 seconden duren op eender welk device voor 90 procent van de gebruikers</t>
+  </si>
+  <si>
+    <t>Inloggen moet automatisch kunnen indien de gebruiker reeds eerder heeft ingelogd binnen de 2 uren</t>
+  </si>
+  <si>
+    <t>Het ophalen van de projectenlijst mag maximaal 5 seconden duren op 90 procent van de devices</t>
+  </si>
+  <si>
+    <t>90 procent van de gebruikers moet binnen 10 seconden een toepasbaar project gevonden hebben</t>
+  </si>
+  <si>
+    <t>90 procent van de gebruikers moet de sorteerfunctie binnen 5 seconden gevonden hebben</t>
+  </si>
+  <si>
+    <t>Gebruikers moeten kunnen zien dat ze een project hebben geliked</t>
+  </si>
+  <si>
+    <t>De detailpagina moet weergeven om welk domein het project betrekking heeft</t>
   </si>
 </sst>
 </file>
@@ -598,6 +595,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,9 +607,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,19 +933,19 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="H2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1198,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>5</v>
@@ -1565,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:F100"/>
+  <dimension ref="D2:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,656 +1575,654 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="28">
+      <c r="D3" s="25">
         <v>1</v>
       </c>
-      <c r="E3" s="28" t="str">
+      <c r="E3" s="25" t="str">
         <f>Gebeurtenissen!C6</f>
         <v>Inloggen</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E8" t="str">
         <f>Gebeurtenissen!C7</f>
         <v>Projectenlijst bekijken</v>
       </c>
-      <c r="F7" s="29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="29" t="s">
-        <v>36</v>
+      <c r="F8" s="26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="29" t="s">
-        <v>37</v>
+      <c r="F9" s="26" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="28">
+      <c r="F10" s="26"/>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="25">
         <v>3</v>
       </c>
-      <c r="E12" s="28" t="str">
+      <c r="E13" s="25" t="str">
         <f>Gebeurtenissen!C8</f>
         <v>Projectenlijst sorteren</v>
       </c>
-      <c r="F12" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28" t="s">
-        <v>39</v>
+      <c r="F13" s="25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28" t="s">
-        <v>40</v>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28" t="s">
-        <v>41</v>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17">
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18">
         <v>4</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E18" t="str">
         <f>Gebeurtenissen!C9</f>
         <v>Projecten filteren</v>
       </c>
-      <c r="F17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="28">
-        <v>5</v>
-      </c>
-      <c r="E20" s="28" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="25">
+        <v>5</v>
+      </c>
+      <c r="E21" s="25" t="str">
         <f>Gebeurtenissen!C10</f>
         <v>Projecten zoeken</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28" t="s">
-        <v>44</v>
+      <c r="F21" s="25" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28" t="s">
-        <v>45</v>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26">
         <v>6</v>
       </c>
-      <c r="E25" t="str">
+      <c r="E26" t="str">
         <f>Gebeurtenissen!C11</f>
         <v>Projecten liken</v>
       </c>
-      <c r="F25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="25">
         <v>7</v>
       </c>
-      <c r="E29" s="28" t="str">
+      <c r="E30" s="25" t="str">
         <f>Gebeurtenissen!C12</f>
         <v>Projectdetails opvragen</v>
       </c>
-      <c r="F29" s="28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28" t="s">
-        <v>50</v>
+      <c r="F30" s="25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28" t="s">
-        <v>51</v>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28" t="s">
-        <v>52</v>
-      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36">
         <v>8</v>
       </c>
-      <c r="E35" t="str">
+      <c r="E36" t="str">
         <f>Gebeurtenissen!C13</f>
         <v>Projectdiscussies bekijken/deelnemen</v>
       </c>
-      <c r="F35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="28">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="25">
         <v>9</v>
       </c>
-      <c r="E41" s="28" t="str">
+      <c r="E42" s="25" t="str">
         <f>Gebeurtenissen!C14</f>
         <v>Projecten delen op sociale media</v>
       </c>
-      <c r="F41" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28" t="s">
-        <v>60</v>
+      <c r="F42" s="25" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="29">
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="26">
         <v>10</v>
       </c>
-      <c r="E45" s="29" t="str">
+      <c r="E46" s="26" t="str">
         <f>Gebeurtenissen!C15</f>
         <v>Inschrijven op projecten</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29" t="s">
-        <v>64</v>
+      <c r="F46" s="26" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29" t="s">
-        <v>65</v>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29" t="s">
-        <v>66</v>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29" t="s">
-        <v>67</v>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29" t="s">
-        <v>68</v>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="29"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="28">
+      <c r="F52" s="26"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="25">
         <v>11</v>
       </c>
-      <c r="E52" s="28" t="str">
+      <c r="E53" s="25" t="str">
         <f>Gebeurtenissen!C16</f>
         <v>Projecten bewerken</v>
       </c>
-      <c r="F52" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28" t="s">
-        <v>69</v>
+      <c r="F53" s="26" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28" t="s">
-        <v>70</v>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28" t="s">
-        <v>71</v>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28" t="s">
-        <v>72</v>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="29"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D58">
+      <c r="F58" s="26"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59">
         <v>12</v>
       </c>
-      <c r="E58" t="str">
+      <c r="E59" t="str">
         <f>Gebeurtenissen!C17</f>
         <v>Projecten verwijderen</v>
       </c>
-      <c r="F58" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="29" t="s">
-        <v>73</v>
+      <c r="F59" s="26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="29" t="s">
-        <v>74</v>
+      <c r="F60" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F61" s="29" t="s">
-        <v>75</v>
+      <c r="F61" s="26" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F62" s="29" t="s">
-        <v>76</v>
+      <c r="F62" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F63" s="29"/>
+      <c r="F63" s="26" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D64" s="28">
+      <c r="F64" s="26"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="25">
         <v>13</v>
       </c>
-      <c r="E64" s="28" t="str">
+      <c r="E65" s="25" t="str">
         <f>Gebeurtenissen!C18</f>
         <v>Annountsments aanmaken</v>
       </c>
-      <c r="F64" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28" t="s">
-        <v>78</v>
+      <c r="F65" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28" t="s">
-        <v>79</v>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28" t="s">
-        <v>80</v>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F68" s="29"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D69">
+      <c r="F69" s="26"/>
+    </row>
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D70">
         <v>14</v>
       </c>
-      <c r="E69" t="str">
+      <c r="E70" t="str">
         <f>Gebeurtenissen!C19</f>
         <v>Projecten aanmaken</v>
       </c>
-      <c r="F69" s="29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F70" s="29" t="s">
-        <v>83</v>
+      <c r="F70" s="26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F71" s="29" t="s">
-        <v>82</v>
+      <c r="F71" s="26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F72" s="29"/>
+      <c r="F72" s="26" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D73" s="28">
+      <c r="F73" s="26"/>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="25">
         <v>15</v>
       </c>
-      <c r="E73" s="28" t="str">
+      <c r="E74" s="25" t="str">
         <f>Gebeurtenissen!C20</f>
         <v>Milestone-statussen aanpassen</v>
       </c>
-      <c r="F73" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28" t="s">
-        <v>85</v>
+      <c r="F74" s="25" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28" t="s">
-        <v>88</v>
+      <c r="D75" s="25"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="25" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F76" s="29"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="25" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D77" s="28">
+      <c r="F77" s="26"/>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="25">
         <v>16</v>
       </c>
-      <c r="E77" s="28" t="str">
+      <c r="E78" s="25" t="str">
         <f>Gebeurtenissen!C21</f>
         <v>Categorieen definieren</v>
       </c>
-      <c r="F77" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
-      <c r="F78" s="28" t="s">
-        <v>90</v>
+      <c r="F78" s="25" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="28" t="s">
-        <v>91</v>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28" t="s">
-        <v>92</v>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F81" s="29"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D82">
+      <c r="F82" s="26"/>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D83">
         <v>17</v>
       </c>
-      <c r="E82" t="str">
+      <c r="E83" t="str">
         <f>Gebeurtenissen!C22</f>
         <v>Projecten backen</v>
       </c>
-      <c r="F82" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F83" s="29" t="s">
-        <v>94</v>
+      <c r="F83" s="26" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F84" s="29" t="s">
-        <v>95</v>
+      <c r="F84" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F85" s="29" t="s">
-        <v>96</v>
+      <c r="F85" s="26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F86" s="29"/>
+      <c r="F86" s="26" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D87" s="28">
+      <c r="F87" s="26"/>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D88" s="25">
         <v>18</v>
       </c>
-      <c r="E87" s="28" t="str">
+      <c r="E88" s="25" t="str">
         <f>Gebeurtenissen!C23</f>
         <v>Projecten publiek maken</v>
       </c>
-      <c r="F87" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D88" s="28"/>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28" t="s">
-        <v>98</v>
+      <c r="F88" s="25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F89" s="29"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="90" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D90">
+      <c r="F90" s="26"/>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D91">
         <v>19</v>
       </c>
-      <c r="E90" t="str">
+      <c r="E91" t="str">
         <f>Gebeurtenissen!C24</f>
         <v>Inschrijvingen verwijderen</v>
       </c>
-      <c r="F90" s="29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F91" s="29" t="s">
-        <v>100</v>
+      <c r="F91" s="26" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F92" s="29"/>
+      <c r="F92" s="26" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="93" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D93" s="28">
+      <c r="F93" s="26"/>
+    </row>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="25">
         <v>20</v>
       </c>
-      <c r="E93" s="28" t="s">
+      <c r="E94" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F93" s="28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D96">
+      <c r="F94" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D97">
         <v>21</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E97" t="s">
         <v>27</v>
       </c>
-      <c r="F96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F97" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D99" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D100" s="25">
         <v>22</v>
       </c>
-      <c r="E99" s="28" t="s">
+      <c r="E100" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F99" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28" t="s">
-        <v>104</v>
+      <c r="F100" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
116 - Plan van aanpak: Quality assurance ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=116 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/Requirements and FIT criteria.xlsx
+++ b/italent/documents/analyse/Requirements and FIT criteria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8205" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gebeurtenissen" sheetId="2" r:id="rId1"/>
@@ -615,6 +615,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,8 +626,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,11 +921,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1062163648"/>
-        <c:axId val="1062777376"/>
+        <c:axId val="-1891940448"/>
+        <c:axId val="-1891944800"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1062163648"/>
+        <c:axId val="-1891940448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +968,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1062777376"/>
+        <c:crossAx val="-1891944800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1062777376"/>
+        <c:axId val="-1891944800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,7 +1027,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1062163648"/>
+        <c:crossAx val="-1891940448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1985,19 +1985,19 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="H2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2630,16 +2630,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G1" s="31">
+      <c r="G1" s="28">
         <v>42491</v>
       </c>
-      <c r="H1" s="31">
+      <c r="H1" s="28">
         <v>42505</v>
       </c>
-      <c r="I1" s="31">
+      <c r="I1" s="28">
         <v>42522</v>
       </c>
-      <c r="J1" s="31">
+      <c r="J1" s="28">
         <v>42530</v>
       </c>
       <c r="L1" t="s">
@@ -4544,13 +4544,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="140.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.140625" customWidth="1"/>
@@ -4566,28 +4564,28 @@
       <c r="C1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="31">
+      <c r="D1" s="28">
         <v>42491</v>
       </c>
-      <c r="E1" s="31">
+      <c r="E1" s="28">
         <v>42500</v>
       </c>
-      <c r="F1" s="31">
+      <c r="F1" s="28">
         <v>42510</v>
       </c>
-      <c r="G1" s="31">
+      <c r="G1" s="28">
         <v>42520</v>
       </c>
-      <c r="H1" s="31">
+      <c r="H1" s="28">
         <v>42522</v>
       </c>
-      <c r="I1" s="31">
+      <c r="I1" s="28">
         <v>42531</v>
       </c>
-      <c r="J1" s="31">
+      <c r="J1" s="28">
         <v>42541</v>
       </c>
-      <c r="K1" s="31"/>
+      <c r="K1" s="28"/>
       <c r="L1" t="s">
         <v>105</v>
       </c>
@@ -4609,7 +4607,7 @@
         <v>30</v>
       </c>
       <c r="L3">
-        <f>IF(B3&lt;&gt;"",1,"")</f>
+        <f t="shared" ref="L3:L34" si="0">IF(B3&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -4647,7 +4645,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <f>IF(B4&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4670,21 +4668,21 @@
         <v>1</v>
       </c>
       <c r="G5" s="26">
-        <f t="shared" ref="G5:G68" si="0">IF(F5&lt;&gt;"",F5,"")</f>
+        <f t="shared" ref="G5:G68" si="1">IF(F5&lt;&gt;"",F5,"")</f>
         <v>1</v>
       </c>
       <c r="H5" s="26">
         <v>1</v>
       </c>
       <c r="I5" s="26">
-        <f t="shared" ref="I5:I68" si="1">IF(H5&lt;&gt;"",H5,"")</f>
+        <f t="shared" ref="I5:I68" si="2">IF(H5&lt;&gt;"",H5,"")</f>
         <v>1</v>
       </c>
       <c r="J5" s="26">
         <v>1</v>
       </c>
       <c r="L5">
-        <f>IF(B5&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4700,28 +4698,28 @@
         <v>1</v>
       </c>
       <c r="E6" s="26">
-        <f t="shared" ref="E6:E69" si="2">IF(D6&lt;&gt;"",D6,"")</f>
+        <f t="shared" ref="E6:E69" si="3">IF(D6&lt;&gt;"",D6,"")</f>
         <v>1</v>
       </c>
       <c r="F6" s="26">
         <v>1</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H6" s="26">
         <v>1</v>
       </c>
       <c r="I6" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J6" s="26">
         <v>1</v>
       </c>
       <c r="L6">
-        <f>IF(B6&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4737,28 +4735,28 @@
         <v>0</v>
       </c>
       <c r="E7" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
+      <c r="G7" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="26">
+        <v>1</v>
+      </c>
+      <c r="I7" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
-      </c>
-      <c r="G7" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="26">
-        <v>1</v>
-      </c>
-      <c r="I7" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J7" s="26">
         <v>1</v>
       </c>
       <c r="L7">
-        <f>IF(B7&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4767,22 +4765,22 @@
       <c r="B8" s="25"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J8" s="26"/>
       <c r="L8" t="str">
-        <f>IF(B8&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4800,28 +4798,28 @@
         <v>0</v>
       </c>
       <c r="E9" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0</v>
+      </c>
+      <c r="G9" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1</v>
+      </c>
+      <c r="I9" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="26">
-        <v>1</v>
-      </c>
-      <c r="I9" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="26">
         <v>1</v>
       </c>
       <c r="L9">
-        <f>IF(B9&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4836,28 +4834,28 @@
         <v>0</v>
       </c>
       <c r="E10" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0</v>
+      </c>
+      <c r="G10" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="26">
+        <v>1</v>
+      </c>
+      <c r="I10" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="26">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="26">
-        <v>1</v>
-      </c>
-      <c r="I10" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="26">
         <v>1</v>
       </c>
       <c r="L10">
-        <f>IF(B10&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4865,66 +4863,66 @@
       <c r="B11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J11" s="26"/>
       <c r="L11" t="str">
-        <f>IF(B11&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="26"/>
       <c r="E12" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J12" s="26"/>
       <c r="L12" t="str">
-        <f>IF(B12&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" s="26"/>
       <c r="E13" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J13" s="26"/>
       <c r="L13" t="str">
-        <f>IF(B13&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4942,28 +4940,28 @@
         <v>0</v>
       </c>
       <c r="E14" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="26">
+        <v>1</v>
+      </c>
+      <c r="G14" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1</v>
+      </c>
+      <c r="I14" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="26">
-        <v>1</v>
-      </c>
-      <c r="G14" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="26">
-        <v>1</v>
-      </c>
-      <c r="I14" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J14" s="26">
         <v>1</v>
       </c>
       <c r="L14">
-        <f>IF(B14&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4979,28 +4977,28 @@
         <v>0</v>
       </c>
       <c r="E15" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1</v>
+      </c>
+      <c r="I15" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="26">
-        <v>1</v>
-      </c>
-      <c r="G15" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="26">
-        <v>1</v>
-      </c>
-      <c r="I15" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J15" s="26">
         <v>1</v>
       </c>
       <c r="L15">
-        <f>IF(B15&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5016,28 +5014,28 @@
         <v>0</v>
       </c>
       <c r="E16" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="26">
+        <v>1</v>
+      </c>
+      <c r="G16" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="26">
+        <v>1</v>
+      </c>
+      <c r="I16" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>1</v>
-      </c>
-      <c r="G16" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H16" s="26">
-        <v>1</v>
-      </c>
-      <c r="I16" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J16" s="26">
         <v>1</v>
       </c>
       <c r="L16">
-        <f>IF(B16&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5053,28 +5051,28 @@
         <v>0</v>
       </c>
       <c r="E17" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0</v>
+      </c>
+      <c r="G17" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="26">
+        <v>1</v>
+      </c>
+      <c r="I17" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="26">
-        <v>0</v>
-      </c>
-      <c r="G17" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
-      <c r="I17" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J17" s="26">
         <v>1</v>
       </c>
       <c r="L17">
-        <f>IF(B17&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5083,22 +5081,22 @@
       <c r="B18" s="25"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J18" s="26"/>
       <c r="L18" t="str">
-        <f>IF(B18&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5116,28 +5114,28 @@
         <v>0</v>
       </c>
       <c r="E19" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0</v>
+      </c>
+      <c r="G19" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="26">
+        <v>1</v>
+      </c>
+      <c r="I19" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="26">
-        <v>0</v>
-      </c>
-      <c r="G19" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
-        <v>1</v>
-      </c>
-      <c r="I19" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" s="26">
         <v>1</v>
       </c>
       <c r="L19">
-        <f>IF(B19&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5152,50 +5150,50 @@
         <v>0</v>
       </c>
       <c r="E20" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0</v>
+      </c>
+      <c r="G20" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="26">
+        <v>1</v>
+      </c>
+      <c r="I20" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="26">
-        <v>0</v>
-      </c>
-      <c r="G20" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="26">
-        <v>1</v>
-      </c>
-      <c r="I20" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="26">
         <v>1</v>
       </c>
       <c r="L20">
-        <f>IF(B20&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21" s="26"/>
       <c r="E21" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J21" s="26"/>
       <c r="L21" t="str">
-        <f>IF(B21&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5213,28 +5211,28 @@
         <v>0</v>
       </c>
       <c r="E22" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="26">
+        <v>1</v>
+      </c>
+      <c r="G22" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="26">
+        <v>1</v>
+      </c>
+      <c r="I22" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="26">
-        <v>1</v>
-      </c>
-      <c r="G22" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22" s="26">
-        <v>1</v>
-      </c>
-      <c r="I22" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J22" s="26">
         <v>1</v>
       </c>
       <c r="L22">
-        <f>IF(B22&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5250,28 +5248,28 @@
         <v>1</v>
       </c>
       <c r="E23" s="26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="26">
+        <v>1</v>
+      </c>
+      <c r="G23" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="26">
+        <v>1</v>
+      </c>
+      <c r="I23" s="26">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F23" s="26">
-        <v>1</v>
-      </c>
-      <c r="G23" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="26">
-        <v>1</v>
-      </c>
-      <c r="I23" s="26">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="J23" s="26">
         <v>1</v>
       </c>
       <c r="L23">
-        <f>IF(B23&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5287,50 +5285,50 @@
         <v>0</v>
       </c>
       <c r="E24" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1</v>
+      </c>
+      <c r="G24" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="26">
+        <v>1</v>
+      </c>
+      <c r="I24" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="26">
-        <v>1</v>
-      </c>
-      <c r="G24" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H24" s="26">
-        <v>1</v>
-      </c>
-      <c r="I24" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J24" s="26">
         <v>1</v>
       </c>
       <c r="L24">
-        <f>IF(B24&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D25" s="26"/>
       <c r="E25" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J25" s="26"/>
       <c r="L25" t="str">
-        <f>IF(B25&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5348,28 +5346,28 @@
         <v>0</v>
       </c>
       <c r="E26" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26" s="26">
-        <v>1</v>
-      </c>
-      <c r="I26" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J26" s="26">
         <v>1</v>
       </c>
       <c r="L26">
-        <f>IF(B26&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5384,28 +5382,28 @@
         <v>0</v>
       </c>
       <c r="E27" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="26">
+        <v>1</v>
+      </c>
+      <c r="G27" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="26">
+        <v>1</v>
+      </c>
+      <c r="I27" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="26">
-        <v>1</v>
-      </c>
-      <c r="G27" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H27" s="26">
-        <v>1</v>
-      </c>
-      <c r="I27" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="26">
         <v>1</v>
       </c>
       <c r="L27">
-        <f>IF(B27&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5420,48 +5418,48 @@
         <v>0</v>
       </c>
       <c r="E28" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="26">
+        <v>0</v>
+      </c>
+      <c r="G28" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="26">
+        <v>1</v>
+      </c>
+      <c r="I28" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="26">
-        <v>0</v>
-      </c>
-      <c r="G28" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="26">
-        <v>1</v>
-      </c>
-      <c r="I28" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="26"/>
       <c r="L28">
-        <f>IF(B28&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D29" s="26"/>
       <c r="E29" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J29" s="26"/>
       <c r="L29" t="str">
-        <f>IF(B29&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5479,28 +5477,28 @@
         <v>0</v>
       </c>
       <c r="E30" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1</v>
+      </c>
+      <c r="G30" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="26">
+        <v>1</v>
+      </c>
+      <c r="I30" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="26">
-        <v>1</v>
-      </c>
-      <c r="G30" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H30" s="26">
-        <v>1</v>
-      </c>
-      <c r="I30" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J30" s="26">
         <v>1</v>
       </c>
       <c r="L30">
-        <f>IF(B30&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5516,28 +5514,28 @@
         <v>0</v>
       </c>
       <c r="E31" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="26">
+        <v>1</v>
+      </c>
+      <c r="G31" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="26">
+        <v>1</v>
+      </c>
+      <c r="I31" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="26">
-        <v>1</v>
-      </c>
-      <c r="G31" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="26">
-        <v>1</v>
-      </c>
-      <c r="I31" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J31" s="26">
         <v>1</v>
       </c>
       <c r="L31">
-        <f>IF(B31&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5553,28 +5551,28 @@
         <v>0</v>
       </c>
       <c r="E32" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="26">
+        <v>0</v>
+      </c>
+      <c r="G32" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="26">
+        <v>1</v>
+      </c>
+      <c r="I32" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="26">
-        <v>0</v>
-      </c>
-      <c r="G32" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="26">
-        <v>1</v>
-      </c>
-      <c r="I32" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J32" s="26">
         <v>1</v>
       </c>
       <c r="L32">
-        <f>IF(B32&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5585,44 +5583,44 @@
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F33" s="26"/>
       <c r="G33" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J33" s="26"/>
       <c r="L33">
-        <f>IF(B33&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D34" s="26"/>
       <c r="E34" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J34" s="26"/>
       <c r="L34" t="str">
-        <f>IF(B34&lt;&gt;"",1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5640,27 +5638,27 @@
         <v>0</v>
       </c>
       <c r="E35" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="26">
+        <v>1</v>
+      </c>
+      <c r="G35" s="26">
+        <v>0</v>
+      </c>
+      <c r="H35" s="26">
+        <v>1</v>
+      </c>
+      <c r="I35" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="26">
-        <v>1</v>
-      </c>
-      <c r="G35" s="26">
-        <v>0</v>
-      </c>
-      <c r="H35" s="26">
-        <v>1</v>
-      </c>
-      <c r="I35" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J35" s="26">
         <v>1</v>
       </c>
       <c r="L35">
-        <f>IF(B35&lt;&gt;"",1,"")</f>
+        <f t="shared" ref="L35:L66" si="4">IF(B35&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -5675,27 +5673,27 @@
         <v>0</v>
       </c>
       <c r="E36" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="26">
+        <v>1</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0</v>
+      </c>
+      <c r="H36" s="26">
+        <v>1</v>
+      </c>
+      <c r="I36" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="26">
-        <v>1</v>
-      </c>
-      <c r="G36" s="26">
-        <v>0</v>
-      </c>
-      <c r="H36" s="26">
-        <v>1</v>
-      </c>
-      <c r="I36" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J36" s="26">
         <v>1</v>
       </c>
       <c r="L36">
-        <f>IF(B36&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5710,27 +5708,27 @@
         <v>0</v>
       </c>
       <c r="E37" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="26">
+        <v>1</v>
+      </c>
+      <c r="G37" s="26">
+        <v>0</v>
+      </c>
+      <c r="H37" s="26">
+        <v>1</v>
+      </c>
+      <c r="I37" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="26">
-        <v>1</v>
-      </c>
-      <c r="G37" s="26">
-        <v>0</v>
-      </c>
-      <c r="H37" s="26">
-        <v>1</v>
-      </c>
-      <c r="I37" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J37" s="26">
         <v>1</v>
       </c>
       <c r="L37">
-        <f>IF(B37&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5745,50 +5743,50 @@
         <v>0</v>
       </c>
       <c r="E38" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="26">
+        <v>0</v>
+      </c>
+      <c r="G38" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="26">
+        <v>1</v>
+      </c>
+      <c r="I38" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="26">
-        <v>0</v>
-      </c>
-      <c r="G38" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="26">
-        <v>1</v>
-      </c>
-      <c r="I38" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J38" s="26">
         <v>1</v>
       </c>
       <c r="L38">
-        <f>IF(B38&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D39" s="26"/>
       <c r="E39" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F39" s="26"/>
       <c r="G39" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J39" s="26"/>
       <c r="L39" t="str">
-        <f>IF(B39&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -5806,28 +5804,28 @@
         <v>0</v>
       </c>
       <c r="E40" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="26">
+        <v>0</v>
+      </c>
+      <c r="G40" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="26">
+        <v>1</v>
+      </c>
+      <c r="I40" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="26">
-        <v>0</v>
-      </c>
-      <c r="G40" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="26">
-        <v>1</v>
-      </c>
-      <c r="I40" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J40" s="26">
         <v>1</v>
       </c>
       <c r="L40">
-        <f>IF(B40&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5843,28 +5841,28 @@
         <v>0</v>
       </c>
       <c r="E41" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="26">
+        <v>1</v>
+      </c>
+      <c r="G41" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="26">
+        <v>1</v>
+      </c>
+      <c r="I41" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="26">
-        <v>1</v>
-      </c>
-      <c r="G41" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H41" s="26">
-        <v>1</v>
-      </c>
-      <c r="I41" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J41" s="26">
         <v>1</v>
       </c>
       <c r="L41">
-        <f>IF(B41&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5880,50 +5878,50 @@
         <v>0</v>
       </c>
       <c r="E42" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="26">
+        <v>1</v>
+      </c>
+      <c r="G42" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="26">
+        <v>1</v>
+      </c>
+      <c r="I42" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="26">
-        <v>1</v>
-      </c>
-      <c r="G42" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H42" s="26">
-        <v>1</v>
-      </c>
-      <c r="I42" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J42" s="26">
         <v>1</v>
       </c>
       <c r="L42">
-        <f>IF(B42&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D43" s="26"/>
       <c r="E43" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F43" s="26"/>
       <c r="G43" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J43" s="26"/>
       <c r="L43" t="str">
-        <f>IF(B43&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -5936,22 +5934,22 @@
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J44" s="26"/>
       <c r="L44">
-        <f>IF(B44&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5967,28 +5965,28 @@
         <v>0</v>
       </c>
       <c r="E45" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="26">
+        <v>1</v>
+      </c>
+      <c r="G45" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H45" s="26">
+        <v>1</v>
+      </c>
+      <c r="I45" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F45" s="26">
-        <v>1</v>
-      </c>
-      <c r="G45" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H45" s="26">
-        <v>1</v>
-      </c>
-      <c r="I45" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J45" s="26">
         <v>1</v>
       </c>
       <c r="L45">
-        <f>IF(B45&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6004,27 +6002,27 @@
         <v>0</v>
       </c>
       <c r="E46" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="26">
+        <v>1</v>
+      </c>
+      <c r="G46" s="26">
+        <v>0</v>
+      </c>
+      <c r="H46" s="26">
+        <v>1</v>
+      </c>
+      <c r="I46" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="26">
-        <v>1</v>
-      </c>
-      <c r="G46" s="26">
-        <v>0</v>
-      </c>
-      <c r="H46" s="26">
-        <v>1</v>
-      </c>
-      <c r="I46" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J46" s="26">
         <v>1</v>
       </c>
       <c r="L46">
-        <f>IF(B46&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6040,28 +6038,28 @@
         <v>0</v>
       </c>
       <c r="E47" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="26">
+        <v>1</v>
+      </c>
+      <c r="G47" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H47" s="26">
+        <v>1</v>
+      </c>
+      <c r="I47" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="26">
-        <v>1</v>
-      </c>
-      <c r="G47" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H47" s="26">
-        <v>1</v>
-      </c>
-      <c r="I47" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J47" s="26">
         <v>1</v>
       </c>
       <c r="L47">
-        <f>IF(B47&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6077,28 +6075,28 @@
         <v>0</v>
       </c>
       <c r="E48" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="26">
+        <v>0</v>
+      </c>
+      <c r="G48" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="26">
+        <v>1</v>
+      </c>
+      <c r="I48" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="26">
-        <v>0</v>
-      </c>
-      <c r="G48" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="26">
-        <v>1</v>
-      </c>
-      <c r="I48" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J48" s="26">
         <v>1</v>
       </c>
       <c r="L48">
-        <f>IF(B48&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6114,27 +6112,27 @@
         <v>0</v>
       </c>
       <c r="E49" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="26">
+        <v>0</v>
+      </c>
+      <c r="G49" s="26">
+        <v>0</v>
+      </c>
+      <c r="H49" s="26">
+        <v>1</v>
+      </c>
+      <c r="I49" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="26">
-        <v>0</v>
-      </c>
-      <c r="G49" s="26">
-        <v>0</v>
-      </c>
-      <c r="H49" s="26">
-        <v>1</v>
-      </c>
-      <c r="I49" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J49" s="26">
         <v>1</v>
       </c>
       <c r="L49">
-        <f>IF(B49&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6142,22 +6140,22 @@
       <c r="B50" s="26"/>
       <c r="D50" s="26"/>
       <c r="E50" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F50" s="26"/>
       <c r="G50" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J50" s="26"/>
       <c r="L50" t="str">
-        <f>IF(B50&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -6175,28 +6173,28 @@
         <v>1</v>
       </c>
       <c r="E51" s="26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="26">
+        <v>1</v>
+      </c>
+      <c r="G51" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H51" s="26">
+        <v>1</v>
+      </c>
+      <c r="I51" s="26">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F51" s="26">
-        <v>1</v>
-      </c>
-      <c r="G51" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H51" s="26">
-        <v>1</v>
-      </c>
-      <c r="I51" s="26">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="J51" s="26">
         <v>1</v>
       </c>
       <c r="L51">
-        <f>IF(B51&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6212,28 +6210,28 @@
         <v>1</v>
       </c>
       <c r="E52" s="26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F52" s="26">
+        <v>1</v>
+      </c>
+      <c r="G52" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H52" s="26">
+        <v>1</v>
+      </c>
+      <c r="I52" s="26">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F52" s="26">
-        <v>1</v>
-      </c>
-      <c r="G52" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H52" s="26">
-        <v>1</v>
-      </c>
-      <c r="I52" s="26">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="J52" s="26">
         <v>1</v>
       </c>
       <c r="L52">
-        <f>IF(B52&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6249,27 +6247,27 @@
         <v>0</v>
       </c>
       <c r="E53" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="26">
+        <v>1</v>
+      </c>
+      <c r="G53" s="26">
+        <v>1</v>
+      </c>
+      <c r="H53" s="26">
+        <v>1</v>
+      </c>
+      <c r="I53" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F53" s="26">
-        <v>1</v>
-      </c>
-      <c r="G53" s="26">
-        <v>1</v>
-      </c>
-      <c r="H53" s="26">
-        <v>1</v>
-      </c>
-      <c r="I53" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J53" s="26">
         <v>1</v>
       </c>
       <c r="L53">
-        <f>IF(B53&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6285,28 +6283,28 @@
         <v>0</v>
       </c>
       <c r="E54" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="26">
+        <v>0</v>
+      </c>
+      <c r="G54" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H54" s="26">
+        <v>1</v>
+      </c>
+      <c r="I54" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="26">
-        <v>0</v>
-      </c>
-      <c r="G54" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="26">
-        <v>1</v>
-      </c>
-      <c r="I54" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J54" s="26">
         <v>1</v>
       </c>
       <c r="L54">
-        <f>IF(B54&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6322,28 +6320,28 @@
         <v>0</v>
       </c>
       <c r="E55" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="26">
+        <v>0</v>
+      </c>
+      <c r="G55" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H55" s="26">
+        <v>1</v>
+      </c>
+      <c r="I55" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="26">
-        <v>0</v>
-      </c>
-      <c r="G55" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="26">
-        <v>1</v>
-      </c>
-      <c r="I55" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J55" s="26">
         <v>1</v>
       </c>
       <c r="L55">
-        <f>IF(B55&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6351,22 +6349,22 @@
       <c r="B56" s="26"/>
       <c r="D56" s="26"/>
       <c r="E56" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F56" s="26"/>
       <c r="G56" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J56" s="26"/>
       <c r="L56" t="str">
-        <f>IF(B56&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -6384,28 +6382,28 @@
         <v>0</v>
       </c>
       <c r="E57" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="26">
+        <v>0</v>
+      </c>
+      <c r="G57" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H57" s="26">
+        <v>0</v>
+      </c>
+      <c r="I57" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F57" s="26">
-        <v>0</v>
-      </c>
-      <c r="G57" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H57" s="26">
-        <v>0</v>
-      </c>
-      <c r="I57" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J57" s="26">
         <v>1</v>
       </c>
       <c r="L57">
-        <f>IF(B57&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6420,28 +6418,28 @@
         <v>0</v>
       </c>
       <c r="E58" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="26">
+        <v>0</v>
+      </c>
+      <c r="G58" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="26">
+        <v>1</v>
+      </c>
+      <c r="I58" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F58" s="26">
-        <v>0</v>
-      </c>
-      <c r="G58" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H58" s="26">
-        <v>1</v>
-      </c>
-      <c r="I58" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J58" s="26">
         <v>1</v>
       </c>
       <c r="L58">
-        <f>IF(B58&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6456,28 +6454,28 @@
         <v>0</v>
       </c>
       <c r="E59" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="26">
+        <v>0</v>
+      </c>
+      <c r="G59" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="26">
+        <v>1</v>
+      </c>
+      <c r="I59" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F59" s="26">
-        <v>0</v>
-      </c>
-      <c r="G59" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H59" s="26">
-        <v>1</v>
-      </c>
-      <c r="I59" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J59" s="26">
         <v>1</v>
       </c>
       <c r="L59">
-        <f>IF(B59&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6492,28 +6490,28 @@
         <v>0</v>
       </c>
       <c r="E60" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="26">
+        <v>1</v>
+      </c>
+      <c r="G60" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H60" s="26">
+        <v>1</v>
+      </c>
+      <c r="I60" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F60" s="26">
-        <v>1</v>
-      </c>
-      <c r="G60" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H60" s="26">
-        <v>1</v>
-      </c>
-      <c r="I60" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J60" s="26">
         <v>1</v>
       </c>
       <c r="L60">
-        <f>IF(B60&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6528,28 +6526,28 @@
         <v>0</v>
       </c>
       <c r="E61" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="26">
+        <v>1</v>
+      </c>
+      <c r="G61" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H61" s="26">
+        <v>1</v>
+      </c>
+      <c r="I61" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F61" s="26">
-        <v>1</v>
-      </c>
-      <c r="G61" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H61" s="26">
-        <v>1</v>
-      </c>
-      <c r="I61" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J61" s="26">
         <v>1</v>
       </c>
       <c r="L61">
-        <f>IF(B61&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6557,22 +6555,22 @@
       <c r="B62" s="26"/>
       <c r="D62" s="26"/>
       <c r="E62" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F62" s="26"/>
       <c r="G62" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H62" s="26"/>
       <c r="I62" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J62" s="26"/>
       <c r="L62" t="str">
-        <f>IF(B62&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -6590,28 +6588,28 @@
         <v>0</v>
       </c>
       <c r="E63" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="26">
+        <v>0</v>
+      </c>
+      <c r="G63" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H63" s="26">
+        <v>0</v>
+      </c>
+      <c r="I63" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F63" s="26">
-        <v>0</v>
-      </c>
-      <c r="G63" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H63" s="26">
-        <v>0</v>
-      </c>
-      <c r="I63" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J63" s="26">
         <v>0</v>
       </c>
       <c r="L63">
-        <f>IF(B63&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6627,28 +6625,28 @@
         <v>0</v>
       </c>
       <c r="E64" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="26">
+        <v>0</v>
+      </c>
+      <c r="G64" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H64" s="26">
+        <v>0</v>
+      </c>
+      <c r="I64" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F64" s="26">
-        <v>0</v>
-      </c>
-      <c r="G64" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H64" s="26">
-        <v>0</v>
-      </c>
-      <c r="I64" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J64" s="26">
         <v>0</v>
       </c>
       <c r="L64">
-        <f>IF(B64&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6664,28 +6662,28 @@
         <v>0</v>
       </c>
       <c r="E65" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="26">
+        <v>0</v>
+      </c>
+      <c r="G65" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="26">
+        <v>0</v>
+      </c>
+      <c r="I65" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F65" s="26">
-        <v>0</v>
-      </c>
-      <c r="G65" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H65" s="26">
-        <v>0</v>
-      </c>
-      <c r="I65" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J65" s="26">
         <v>0</v>
       </c>
       <c r="L65">
-        <f>IF(B65&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6701,28 +6699,28 @@
         <v>0</v>
       </c>
       <c r="E66" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="26">
+        <v>0</v>
+      </c>
+      <c r="G66" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H66" s="26">
+        <v>0</v>
+      </c>
+      <c r="I66" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F66" s="26">
-        <v>0</v>
-      </c>
-      <c r="G66" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H66" s="26">
-        <v>0</v>
-      </c>
-      <c r="I66" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J66" s="26">
         <v>0</v>
       </c>
       <c r="L66">
-        <f>IF(B66&lt;&gt;"",1,"")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -6730,22 +6728,22 @@
       <c r="B67" s="26"/>
       <c r="D67" s="26"/>
       <c r="E67" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F67" s="26"/>
       <c r="G67" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H67" s="26"/>
       <c r="I67" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J67" s="26"/>
       <c r="L67" t="str">
-        <f>IF(B67&lt;&gt;"",1,"")</f>
+        <f t="shared" ref="L67:L99" si="5">IF(B67&lt;&gt;"",1,"")</f>
         <v/>
       </c>
     </row>
@@ -6763,28 +6761,28 @@
         <v>0</v>
       </c>
       <c r="E68" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F68" s="26">
+        <v>1</v>
+      </c>
+      <c r="G68" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H68" s="26">
+        <v>1</v>
+      </c>
+      <c r="I68" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F68" s="26">
-        <v>1</v>
-      </c>
-      <c r="G68" s="26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H68" s="26">
-        <v>1</v>
-      </c>
-      <c r="I68" s="26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J68" s="26">
         <v>1</v>
       </c>
       <c r="L68">
-        <f>IF(B68&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6799,28 +6797,28 @@
         <v>0</v>
       </c>
       <c r="E69" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F69" s="26">
         <v>1</v>
       </c>
       <c r="G69" s="26">
-        <f t="shared" ref="G69:G99" si="3">IF(F69&lt;&gt;"",F69,"")</f>
+        <f t="shared" ref="G69:G99" si="6">IF(F69&lt;&gt;"",F69,"")</f>
         <v>1</v>
       </c>
       <c r="H69" s="26">
         <v>1</v>
       </c>
       <c r="I69" s="26">
-        <f t="shared" ref="I69:I99" si="4">IF(H69&lt;&gt;"",H69,"")</f>
+        <f t="shared" ref="I69:I99" si="7">IF(H69&lt;&gt;"",H69,"")</f>
         <v>1</v>
       </c>
       <c r="J69" s="26">
         <v>1</v>
       </c>
       <c r="L69">
-        <f>IF(B69&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6835,28 +6833,28 @@
         <v>0</v>
       </c>
       <c r="E70" s="26">
-        <f t="shared" ref="E70:E99" si="5">IF(D70&lt;&gt;"",D70,"")</f>
+        <f t="shared" ref="E70:E99" si="8">IF(D70&lt;&gt;"",D70,"")</f>
         <v>0</v>
       </c>
       <c r="F70" s="26">
         <v>1</v>
       </c>
       <c r="G70" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H70" s="26">
         <v>1</v>
       </c>
       <c r="I70" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J70" s="26">
         <v>1</v>
       </c>
       <c r="L70">
-        <f>IF(B70&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6864,22 +6862,22 @@
       <c r="B71" s="26"/>
       <c r="D71" s="26"/>
       <c r="E71" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H71" s="26"/>
       <c r="I71" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J71" s="26"/>
       <c r="L71" t="str">
-        <f>IF(B71&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6897,28 +6895,28 @@
         <v>0</v>
       </c>
       <c r="E72" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F72" s="26">
+        <v>0</v>
+      </c>
+      <c r="G72" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H72" s="26">
+        <v>0</v>
+      </c>
+      <c r="I72" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J72" s="26">
+        <v>1</v>
+      </c>
+      <c r="L72">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F72" s="26">
-        <v>0</v>
-      </c>
-      <c r="G72" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H72" s="26">
-        <v>0</v>
-      </c>
-      <c r="I72" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J72" s="26">
-        <v>1</v>
-      </c>
-      <c r="L72">
-        <f>IF(B72&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -6934,28 +6932,28 @@
         <v>0</v>
       </c>
       <c r="E73" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="26">
+        <v>0</v>
+      </c>
+      <c r="G73" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H73" s="26">
+        <v>0</v>
+      </c>
+      <c r="I73" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J73" s="26">
+        <v>1</v>
+      </c>
+      <c r="L73">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F73" s="26">
-        <v>0</v>
-      </c>
-      <c r="G73" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H73" s="26">
-        <v>0</v>
-      </c>
-      <c r="I73" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J73" s="26">
-        <v>1</v>
-      </c>
-      <c r="L73">
-        <f>IF(B73&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -6971,28 +6969,28 @@
         <v>0</v>
       </c>
       <c r="E74" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F74" s="26">
+        <v>0</v>
+      </c>
+      <c r="G74" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H74" s="26">
+        <v>0</v>
+      </c>
+      <c r="I74" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J74" s="26">
+        <v>1</v>
+      </c>
+      <c r="L74">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F74" s="26">
-        <v>0</v>
-      </c>
-      <c r="G74" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H74" s="26">
-        <v>0</v>
-      </c>
-      <c r="I74" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J74" s="26">
-        <v>1</v>
-      </c>
-      <c r="L74">
-        <f>IF(B74&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7000,22 +6998,22 @@
       <c r="B75" s="26"/>
       <c r="D75" s="26"/>
       <c r="E75" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F75" s="26"/>
       <c r="G75" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H75" s="26"/>
       <c r="I75" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J75" s="26"/>
       <c r="L75" t="str">
-        <f>IF(B75&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7033,28 +7031,28 @@
         <v>0</v>
       </c>
       <c r="E76" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F76" s="26">
+        <v>1</v>
+      </c>
+      <c r="G76" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H76" s="26">
+        <v>1</v>
+      </c>
+      <c r="I76" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J76" s="26">
+        <v>1</v>
+      </c>
+      <c r="L76">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F76" s="26">
-        <v>1</v>
-      </c>
-      <c r="G76" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H76" s="26">
-        <v>1</v>
-      </c>
-      <c r="I76" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J76" s="26">
-        <v>1</v>
-      </c>
-      <c r="L76">
-        <f>IF(B76&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7070,28 +7068,28 @@
         <v>0</v>
       </c>
       <c r="E77" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F77" s="26">
+        <v>1</v>
+      </c>
+      <c r="G77" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H77" s="26">
+        <v>1</v>
+      </c>
+      <c r="I77" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J77" s="26">
+        <v>1</v>
+      </c>
+      <c r="L77">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F77" s="26">
-        <v>1</v>
-      </c>
-      <c r="G77" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H77" s="26">
-        <v>1</v>
-      </c>
-      <c r="I77" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J77" s="26">
-        <v>1</v>
-      </c>
-      <c r="L77">
-        <f>IF(B77&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7107,28 +7105,28 @@
         <v>1</v>
       </c>
       <c r="E78" s="26">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F78" s="26">
+        <v>1</v>
+      </c>
+      <c r="G78" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H78" s="26">
+        <v>1</v>
+      </c>
+      <c r="I78" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J78" s="26">
+        <v>1</v>
+      </c>
+      <c r="L78">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="F78" s="26">
-        <v>1</v>
-      </c>
-      <c r="G78" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H78" s="26">
-        <v>1</v>
-      </c>
-      <c r="I78" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J78" s="26">
-        <v>1</v>
-      </c>
-      <c r="L78">
-        <f>IF(B78&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7144,28 +7142,28 @@
         <v>0</v>
       </c>
       <c r="E79" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="26">
+        <v>1</v>
+      </c>
+      <c r="G79" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H79" s="26">
+        <v>1</v>
+      </c>
+      <c r="I79" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J79" s="26">
+        <v>1</v>
+      </c>
+      <c r="L79">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F79" s="26">
-        <v>1</v>
-      </c>
-      <c r="G79" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H79" s="26">
-        <v>1</v>
-      </c>
-      <c r="I79" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J79" s="26">
-        <v>1</v>
-      </c>
-      <c r="L79">
-        <f>IF(B79&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7173,22 +7171,22 @@
       <c r="B80" s="26"/>
       <c r="D80" s="26"/>
       <c r="E80" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F80" s="26"/>
       <c r="G80" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H80" s="26"/>
       <c r="I80" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J80" s="26"/>
       <c r="L80" t="str">
-        <f>IF(B80&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7206,28 +7204,28 @@
         <v>0</v>
       </c>
       <c r="E81" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="26">
+        <v>0</v>
+      </c>
+      <c r="G81" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H81" s="26">
+        <v>1</v>
+      </c>
+      <c r="I81" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J81" s="26">
+        <v>1</v>
+      </c>
+      <c r="L81">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F81" s="26">
-        <v>0</v>
-      </c>
-      <c r="G81" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H81" s="26">
-        <v>1</v>
-      </c>
-      <c r="I81" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J81" s="26">
-        <v>1</v>
-      </c>
-      <c r="L81">
-        <f>IF(B81&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7242,28 +7240,28 @@
         <v>0</v>
       </c>
       <c r="E82" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="26">
+        <v>0</v>
+      </c>
+      <c r="G82" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H82" s="26">
+        <v>1</v>
+      </c>
+      <c r="I82" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J82" s="26">
+        <v>1</v>
+      </c>
+      <c r="L82">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F82" s="26">
-        <v>0</v>
-      </c>
-      <c r="G82" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H82" s="26">
-        <v>1</v>
-      </c>
-      <c r="I82" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J82" s="26">
-        <v>1</v>
-      </c>
-      <c r="L82">
-        <f>IF(B82&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7278,28 +7276,28 @@
         <v>0</v>
       </c>
       <c r="E83" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="26">
+        <v>0</v>
+      </c>
+      <c r="G83" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H83" s="26">
+        <v>1</v>
+      </c>
+      <c r="I83" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J83" s="26">
+        <v>1</v>
+      </c>
+      <c r="L83">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F83" s="26">
-        <v>0</v>
-      </c>
-      <c r="G83" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H83" s="26">
-        <v>1</v>
-      </c>
-      <c r="I83" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J83" s="26">
-        <v>1</v>
-      </c>
-      <c r="L83">
-        <f>IF(B83&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7314,28 +7312,28 @@
         <v>0</v>
       </c>
       <c r="E84" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F84" s="26">
+        <v>0</v>
+      </c>
+      <c r="G84" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H84" s="26">
+        <v>1</v>
+      </c>
+      <c r="I84" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J84" s="26">
+        <v>1</v>
+      </c>
+      <c r="L84">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F84" s="26">
-        <v>0</v>
-      </c>
-      <c r="G84" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H84" s="26">
-        <v>1</v>
-      </c>
-      <c r="I84" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J84" s="26">
-        <v>1</v>
-      </c>
-      <c r="L84">
-        <f>IF(B84&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7343,22 +7341,22 @@
       <c r="B85" s="26"/>
       <c r="D85" s="26"/>
       <c r="E85" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F85" s="26"/>
       <c r="G85" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H85" s="26"/>
       <c r="I85" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J85" s="26"/>
       <c r="L85" t="str">
-        <f>IF(B85&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7376,28 +7374,28 @@
         <v>0</v>
       </c>
       <c r="E86" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F86" s="26">
+        <v>0</v>
+      </c>
+      <c r="G86" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H86" s="26">
+        <v>1</v>
+      </c>
+      <c r="I86" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J86" s="26">
+        <v>1</v>
+      </c>
+      <c r="L86">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F86" s="26">
-        <v>0</v>
-      </c>
-      <c r="G86" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H86" s="26">
-        <v>1</v>
-      </c>
-      <c r="I86" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J86" s="26">
-        <v>1</v>
-      </c>
-      <c r="L86">
-        <f>IF(B86&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7413,28 +7411,28 @@
         <v>0</v>
       </c>
       <c r="E87" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="26">
+        <v>0</v>
+      </c>
+      <c r="G87" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H87" s="26">
+        <v>1</v>
+      </c>
+      <c r="I87" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J87" s="26">
+        <v>1</v>
+      </c>
+      <c r="L87">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F87" s="26">
-        <v>0</v>
-      </c>
-      <c r="G87" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H87" s="26">
-        <v>1</v>
-      </c>
-      <c r="I87" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J87" s="26">
-        <v>1</v>
-      </c>
-      <c r="L87">
-        <f>IF(B87&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7442,22 +7440,22 @@
       <c r="B88" s="26"/>
       <c r="D88" s="26"/>
       <c r="E88" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F88" s="26"/>
       <c r="G88" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H88" s="26"/>
       <c r="I88" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J88" s="26"/>
       <c r="L88" t="str">
-        <f>IF(B88&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7470,22 +7468,22 @@
       </c>
       <c r="D89" s="26"/>
       <c r="E89" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F89" s="26"/>
       <c r="G89" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H89" s="26"/>
       <c r="I89" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J89" s="26"/>
       <c r="L89">
-        <f>IF(B89&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7500,28 +7498,28 @@
         <v>0</v>
       </c>
       <c r="E90" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F90" s="26">
+        <v>0</v>
+      </c>
+      <c r="G90" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H90" s="26">
+        <v>1</v>
+      </c>
+      <c r="I90" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J90" s="26">
+        <v>1</v>
+      </c>
+      <c r="L90">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F90" s="26">
-        <v>0</v>
-      </c>
-      <c r="G90" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H90" s="26">
-        <v>1</v>
-      </c>
-      <c r="I90" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J90" s="26">
-        <v>1</v>
-      </c>
-      <c r="L90">
-        <f>IF(B90&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7534,28 +7532,28 @@
         <v>0</v>
       </c>
       <c r="E91" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F91" s="26">
+        <v>0</v>
+      </c>
+      <c r="G91" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H91" s="26">
+        <v>1</v>
+      </c>
+      <c r="I91" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J91" s="26">
+        <v>1</v>
+      </c>
+      <c r="L91" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F91" s="26">
-        <v>0</v>
-      </c>
-      <c r="G91" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H91" s="26">
-        <v>1</v>
-      </c>
-      <c r="I91" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J91" s="26">
-        <v>1</v>
-      </c>
-      <c r="L91" t="str">
-        <f>IF(B91&lt;&gt;"",1,"")</f>
         <v/>
       </c>
     </row>
@@ -7573,28 +7571,28 @@
         <v>0</v>
       </c>
       <c r="E92" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F92" s="26">
+        <v>1</v>
+      </c>
+      <c r="G92" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H92" s="26">
+        <v>1</v>
+      </c>
+      <c r="I92" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J92" s="26">
+        <v>1</v>
+      </c>
+      <c r="L92">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F92" s="26">
-        <v>1</v>
-      </c>
-      <c r="G92" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H92" s="26">
-        <v>1</v>
-      </c>
-      <c r="I92" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J92" s="26">
-        <v>1</v>
-      </c>
-      <c r="L92">
-        <f>IF(B92&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7610,50 +7608,50 @@
         <v>0</v>
       </c>
       <c r="E93" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F93" s="26">
+        <v>0</v>
+      </c>
+      <c r="G93" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H93" s="26">
+        <v>0</v>
+      </c>
+      <c r="I93" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J93" s="26">
+        <v>0</v>
+      </c>
+      <c r="L93">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F93" s="26">
-        <v>0</v>
-      </c>
-      <c r="G93" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H93" s="26">
-        <v>0</v>
-      </c>
-      <c r="I93" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="26">
-        <v>0</v>
-      </c>
-      <c r="L93">
-        <f>IF(B93&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D94" s="26"/>
       <c r="E94" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F94" s="26"/>
       <c r="G94" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H94" s="26"/>
       <c r="I94" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J94" s="26"/>
       <c r="L94" t="str">
-        <f>IF(B94&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7671,28 +7669,28 @@
         <v>0</v>
       </c>
       <c r="E95" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F95" s="26">
+        <v>1</v>
+      </c>
+      <c r="G95" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H95" s="26">
+        <v>1</v>
+      </c>
+      <c r="I95" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J95" s="26">
+        <v>1</v>
+      </c>
+      <c r="L95">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F95" s="26">
-        <v>1</v>
-      </c>
-      <c r="G95" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H95" s="26">
-        <v>1</v>
-      </c>
-      <c r="I95" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J95" s="26">
-        <v>1</v>
-      </c>
-      <c r="L95">
-        <f>IF(B95&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7707,50 +7705,50 @@
         <v>0</v>
       </c>
       <c r="E96" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="26">
+        <v>1</v>
+      </c>
+      <c r="G96" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H96" s="26">
+        <v>1</v>
+      </c>
+      <c r="I96" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J96" s="26">
+        <v>1</v>
+      </c>
+      <c r="L96">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F96" s="26">
-        <v>1</v>
-      </c>
-      <c r="G96" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H96" s="26">
-        <v>1</v>
-      </c>
-      <c r="I96" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J96" s="26">
-        <v>1</v>
-      </c>
-      <c r="L96">
-        <f>IF(B96&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D97" s="26"/>
       <c r="E97" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F97" s="26"/>
       <c r="G97" s="26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H97" s="26"/>
       <c r="I97" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J97" s="26"/>
       <c r="L97" t="str">
-        <f>IF(B97&lt;&gt;"",1,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -7768,28 +7766,28 @@
         <v>0</v>
       </c>
       <c r="E98" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="26">
+        <v>1</v>
+      </c>
+      <c r="G98" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H98" s="26">
+        <v>1</v>
+      </c>
+      <c r="I98" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J98" s="26">
+        <v>1</v>
+      </c>
+      <c r="L98">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F98" s="26">
-        <v>1</v>
-      </c>
-      <c r="G98" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H98" s="26">
-        <v>1</v>
-      </c>
-      <c r="I98" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J98" s="26">
-        <v>1</v>
-      </c>
-      <c r="L98">
-        <f>IF(B98&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7805,28 +7803,28 @@
         <v>0</v>
       </c>
       <c r="E99" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="26">
+        <v>1</v>
+      </c>
+      <c r="G99" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H99" s="26">
+        <v>1</v>
+      </c>
+      <c r="I99" s="26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J99" s="26">
+        <v>1</v>
+      </c>
+      <c r="L99">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F99" s="26">
-        <v>1</v>
-      </c>
-      <c r="G99" s="26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H99" s="26">
-        <v>1</v>
-      </c>
-      <c r="I99" s="26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J99" s="26">
-        <v>1</v>
-      </c>
-      <c r="L99">
-        <f>IF(B99&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -7849,31 +7847,31 @@
         <v>7</v>
       </c>
       <c r="E101">
-        <f t="shared" ref="E101:J101" si="6">SUM(E4:E100)</f>
+        <f t="shared" ref="E101:J101" si="9">SUM(E4:E100)</f>
         <v>7</v>
       </c>
       <c r="F101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>38</v>
       </c>
       <c r="G101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="H101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="I101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="J101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="L101">
-        <f t="shared" ref="L101" si="7">SUM(L3:L99)</f>
+        <f t="shared" ref="L101" si="10">SUM(L3:L99)</f>
         <v>74</v>
       </c>
     </row>
@@ -7896,7 +7894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -7913,37 +7911,37 @@
       <c r="B2" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="30" t="str">
+      <c r="C2" s="27" t="str">
         <f>'Test overview'!C1</f>
         <v>20-04-2016</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="27">
         <f>'Test overview'!D1</f>
         <v>42491</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="27">
         <f>'Test overview'!E1</f>
         <v>42500</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="27">
         <f>'Test overview'!F1</f>
         <v>42510</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="27">
         <f>'Test overview'!G1</f>
         <v>42520</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="27">
         <f>'Test overview'!H1</f>
         <v>42522</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="27">
         <f>'Test overview'!I1</f>
         <v>42531</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -7987,7 +7985,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:J4" si="0">D5-D3</f>
+        <f t="shared" ref="D4:I4" si="0">D5-D3</f>
         <v>8</v>
       </c>
       <c r="E4">

</xml_diff>